<commit_message>
DataProvider annotation  was added
</commit_message>
<xml_diff>
--- a/src/test/resources/VytrackTestData.xlsx
+++ b/src/test/resources/VytrackTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhammet/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhammet/Desktop/CybertekKendiCalismam/Selenium/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B795D8-0BB8-4A4B-8C9F-0397977DEC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB07DEF-3D21-2E4C-B517-D289CE59FECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{A7B5D676-3A9D-C34E-A2AB-F182BC41B75D}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>UserUser123</t>
   </si>
   <si>
-    <t xml:space="preserve">John </t>
-  </si>
-  <si>
     <t>Doe</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>Rempel</t>
   </si>
   <si>
-    <t>Turmer</t>
-  </si>
-  <si>
     <t>Considine</t>
   </si>
   <si>
@@ -158,6 +152,12 @@
   </si>
   <si>
     <t>Parisian</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Turner</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,10 +549,10 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -563,10 +563,10 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -577,10 +577,10 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -591,10 +591,10 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -605,10 +605,10 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
         <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -619,10 +619,10 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -633,10 +633,10 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -647,10 +647,10 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -661,10 +661,10 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -675,10 +675,10 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -689,10 +689,10 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -703,10 +703,10 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -717,10 +717,10 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>